<commit_message>
Removed highlighting of cells
</commit_message>
<xml_diff>
--- a/reconciliation/Reconciliation table (brief version).xlsx
+++ b/reconciliation/Reconciliation table (brief version).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobba\Dropbox\work\z_research\OpenMetaAnalysis\_Methods paper\Reconciliation tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobba\Documents\GitHub\openMetaAnalysis\openMetaAnalysis.github.io\reconciliation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BF7ADD-3EA3-49BB-8294-F745939FAB38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9A99C2D-9502-465B-9AFA-4C0E0A8FAAA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2412" yWindow="1272" windowWidth="20340" windowHeight="11940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1092" yWindow="60" windowWidth="23040" windowHeight="11940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reconciliation table combined" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="98">
   <si>
     <t>Heterogeneity</t>
   </si>
@@ -221,121 +221,6 @@
     <t>Abbreviations: RR: Risk Ratio; CI: Confidence Interval</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>= 19</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>= 42</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>= 17</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>= 37</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>= 23</t>
-    </r>
-  </si>
-  <si>
     <t>0.96 (0.85-1.08)</t>
   </si>
   <si>
@@ -432,53 +317,7 @@
 PMID 31423390 </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>= 5</t>
-    </r>
-  </si>
-  <si>
     <t>Septic shock only</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>= 10</t>
-    </r>
   </si>
   <si>
     <t>0.93 (0.86-1.01)</t>
@@ -487,47 +326,10 @@
     <t>Keh</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>= 23</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>e</t>
-    </r>
-  </si>
-  <si>
     <t>Reconciliation of studies included &amp; conclusions with prior systematic reviews</t>
   </si>
   <si>
     <t>0.92 (0.85-0.99)</t>
-  </si>
-  <si>
-    <t>f: systemic hydrocortisone in any form, dose, route, and duration, whether it was used alone or in combination with other forms of steroids, with or without tapering</t>
   </si>
   <si>
     <r>
@@ -553,52 +355,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>: short-term mortality was defined as mortality within 90 days after randomization</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>= 35</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>= 33</t>
     </r>
   </si>
   <si>
@@ -651,44 +407,10 @@
     </r>
   </si>
   <si>
-    <t>g: 12 eligible/new studies were included through an updated search; an updated systematic review and meta-analysis based on Annane, 2015, PMID: 26633262 which contributed 30 eligible studies</t>
-  </si>
-  <si>
-    <r>
-      <t>h: trials including children were not in the analysis for short-term mortality; h</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: 9 eligible/new studies were included through an updated search; an updated systematic review and meta-analysis based on Annane, 2009, PMID: 19509383</t>
-    </r>
-  </si>
-  <si>
     <t>c: differences in the number of studies included in the systematic reviews and meta-analyses are due to variations in eligibility criteria and search strategy opted in each systematic review</t>
   </si>
   <si>
     <t>Note: No network meta-analyses were included</t>
-  </si>
-  <si>
-    <t>N: total number of studies included in the systematic review; 
-n: number of studies included in the analysis for short-term mortality
-↓: significant decrease; ↑: significant increase; ↔: no significant change</t>
   </si>
   <si>
     <t>Population benefited</t>
@@ -706,14 +428,295 @@
     <t>Septic shock on pressors</t>
   </si>
   <si>
-    <t>Studies included</t>
+    <r>
+      <t>Studies included</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>b,c</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N: total number of studies included in the systematic review; n: number of studies included in the analysis for short-term mortality</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+↓: significant decrease; ↑: significant increase; ↔: no significant change</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= 9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= 5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= 23</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= 34</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= 18</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= 36</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= 22</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= 16</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= 23</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= 6</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -789,28 +792,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="52">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -1054,15 +1064,6 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -1253,58 +1254,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -1380,43 +1329,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -1475,19 +1387,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -1497,10 +1444,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1510,62 +1455,150 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1580,22 +1613,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1603,51 +1636,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1658,61 +1646,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4712,7 +4647,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5693991" y="3155201"/>
+          <a:off x="5696737" y="2157647"/>
           <a:ext cx="93382" cy="93383"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
@@ -4754,13 +4689,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>782262</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>144089</xdr:rowOff>
+      <xdr:rowOff>132401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>875644</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>237472</xdr:rowOff>
+      <xdr:rowOff>225784</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4775,7 +4710,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5834247" y="4794530"/>
+          <a:off x="5842783" y="2154272"/>
           <a:ext cx="93382" cy="93383"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
@@ -5006,13 +4941,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>490646</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>142186</xdr:rowOff>
+      <xdr:rowOff>136342</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>584028</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>235569</xdr:rowOff>
+      <xdr:rowOff>229725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5027,7 +4962,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5542631" y="4792627"/>
+          <a:off x="5551167" y="2158213"/>
           <a:ext cx="93382" cy="93383"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
@@ -7370,37 +7305,37 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>46511</xdr:colOff>
+      <xdr:colOff>44051</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>35829</xdr:rowOff>
+      <xdr:rowOff>49713</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>149232</xdr:colOff>
+      <xdr:colOff>146772</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>129211</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="235" name="Rectangle 234">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1E02C42-CABD-40BB-9329-666E3B50BA9B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4791900" y="1159437"/>
+      <xdr:rowOff>143095</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="236" name="Rectangle 235">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED1A03AF-4C9D-4B8A-A2A1-3C38E5E2BBF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7068739" y="1881953"/>
           <a:ext cx="102721" cy="93382"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="92D050"/>
+          <a:srgbClr val="00B050"/>
         </a:solidFill>
       </xdr:spPr>
       <xdr:style>
@@ -7433,37 +7368,37 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>189572</xdr:colOff>
+      <xdr:colOff>184362</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>36484</xdr:rowOff>
+      <xdr:rowOff>48873</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292293</xdr:colOff>
+      <xdr:colOff>287083</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>129866</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="236" name="Rectangle 235">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED1A03AF-4C9D-4B8A-A2A1-3C38E5E2BBF6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4934961" y="1160092"/>
-          <a:ext cx="102721" cy="93382"/>
+      <xdr:rowOff>140040</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="239" name="Rectangle 238">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C43243C-D1A4-4D75-9C14-F0326A54630D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7209050" y="1881113"/>
+          <a:ext cx="102721" cy="91167"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="00B050"/>
+          <a:srgbClr val="002060"/>
         </a:solidFill>
       </xdr:spPr>
       <xdr:style>
@@ -7496,220 +7431,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>333939</xdr:colOff>
+      <xdr:colOff>334303</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>38568</xdr:rowOff>
+      <xdr:rowOff>44277</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>436660</xdr:colOff>
+      <xdr:colOff>437024</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>133405</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="237" name="Rectangle 236">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{375D2307-43C1-4E06-84AB-CE9610C75A33}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8201589" y="2619843"/>
+      <xdr:rowOff>139114</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="246" name="Rectangle 245">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47CD961A-5414-4343-9B2E-B2138BADBC54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7358991" y="1876517"/>
           <a:ext cx="102721" cy="94837"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="00B0F0"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>475404</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>38951</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>578125</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>130118</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="239" name="Rectangle 238">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C43243C-D1A4-4D75-9C14-F0326A54630D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7495329" y="2867876"/>
-          <a:ext cx="102721" cy="91167"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="002060"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>627804</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>38378</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>730525</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>129478</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="245" name="Rectangle 244">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8EAF3E6-9AA3-4A14-A855-6AF2391E6352}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7627720" y="2857522"/>
-          <a:ext cx="102721" cy="91100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="7030A0"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>770866</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>35359</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>873587</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>121574</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="246" name="Rectangle 245">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47CD961A-5414-4343-9B2E-B2138BADBC54}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7770782" y="2854503"/>
-          <a:ext cx="102721" cy="86215"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7750,80 +7496,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>46048</xdr:colOff>
+      <xdr:colOff>484258</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>172163</xdr:rowOff>
+      <xdr:rowOff>48107</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>148769</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>77327</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="248" name="Rectangle 247">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4141429D-4679-4CEA-9D1F-23771DC7B453}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4791437" y="1295771"/>
-          <a:ext cx="102721" cy="93382"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent4">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>193216</xdr:colOff>
+      <xdr:colOff>586979</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>175991</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>295937</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>81155</xdr:rowOff>
+      <xdr:rowOff>136277</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7838,8 +7519,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4938605" y="1299599"/>
-          <a:ext cx="102721" cy="93382"/>
+          <a:off x="7508946" y="1880347"/>
+          <a:ext cx="102721" cy="88170"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7880,37 +7561,37 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>339953</xdr:colOff>
+      <xdr:colOff>640430</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>175344</xdr:rowOff>
+      <xdr:rowOff>43403</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>442674</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>80508</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="251" name="Rectangle 250">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1930F652-420A-49CC-83C3-5714B7CEC76D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5085342" y="1298952"/>
-          <a:ext cx="102721" cy="93382"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="tx1"/>
+      <xdr:colOff>733812</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>136786</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="268" name="Isosceles Triangle 267">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62A9B916-784A-4D14-BA24-BA8CC7F000F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7654656" y="1880652"/>
+          <a:ext cx="93382" cy="93383"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="7030A0"/>
         </a:solidFill>
       </xdr:spPr>
       <xdr:style>
@@ -7943,462 +7624,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>489149</xdr:colOff>
+      <xdr:colOff>789390</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>175615</xdr:rowOff>
+      <xdr:rowOff>42861</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>591870</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>80779</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="253" name="Rectangle 252">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6984BEBF-0679-459D-A1A8-210EB337F75E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5234538" y="1299223"/>
-          <a:ext cx="102721" cy="93382"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent5">
-            <a:lumMod val="40000"/>
-            <a:lumOff val="60000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>637543</xdr:colOff>
+      <xdr:colOff>882772</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>174344</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>740264</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>79508</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="255" name="Rectangle 254">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{422BC115-DE37-440F-80A4-F696D647DE7E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8505193" y="2755619"/>
-          <a:ext cx="102721" cy="95664"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent4">
-            <a:lumMod val="40000"/>
-            <a:lumOff val="60000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>773588</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>172881</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>866970</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>78046</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="260" name="Isosceles Triangle 259">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8516780-84D1-487F-B499-209419B57DA0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8641238" y="2754156"/>
-          <a:ext cx="93382" cy="95665"/>
-        </a:xfrm>
-        <a:prstGeom prst="triangle">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFC000"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>48910</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>133417</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>142292</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>226800</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="264" name="Isosceles Triangle 263">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDEC1AD8-7571-4418-8FC1-5CCC98E7CBFB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7068835" y="3152842"/>
-          <a:ext cx="93382" cy="93383"/>
-        </a:xfrm>
-        <a:prstGeom prst="triangle">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="00B050"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>181989</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>130123</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>275371</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>223506</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="266" name="Isosceles Triangle 265">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B09250D7-80A8-4E25-99A9-AB701887FCCC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7201914" y="3149548"/>
-          <a:ext cx="93382" cy="93383"/>
-        </a:xfrm>
-        <a:prstGeom prst="triangle">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="0070C0"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>320289</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>130731</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>413671</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>224114</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="267" name="Isosceles Triangle 266">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBA63333-D0C3-4E87-A4AF-ABFF2729FBC5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5065678" y="1442557"/>
-          <a:ext cx="93382" cy="93383"/>
-        </a:xfrm>
-        <a:prstGeom prst="triangle">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="002060"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>459026</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>129393</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>552408</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>222776</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="268" name="Isosceles Triangle 267">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62A9B916-784A-4D14-BA24-BA8CC7F000F9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5204415" y="1441219"/>
-          <a:ext cx="93382" cy="93383"/>
-        </a:xfrm>
-        <a:prstGeom prst="triangle">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="7030A0"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>601290</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>129530</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>694672</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>222913</xdr:rowOff>
+      <xdr:rowOff>136244</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8413,7 +7647,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7621215" y="3148955"/>
+          <a:off x="7803616" y="1880110"/>
           <a:ext cx="93382" cy="93383"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
@@ -13950,76 +13184,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>351998</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>46118</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>454719</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>139500</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="256" name="Rectangle 255">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{104EB235-F6E5-4B2B-9CFC-4E66E651E796}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2466548" y="2875043"/>
-          <a:ext cx="102721" cy="93382"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FF7D2D"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>505135</xdr:colOff>
+      <xdr:colOff>361060</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>46533</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>598517</xdr:colOff>
+      <xdr:colOff>454442</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>139916</xdr:rowOff>
     </xdr:to>
@@ -14036,7 +13207,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2619685" y="2875458"/>
+          <a:off x="2482173" y="1887499"/>
           <a:ext cx="93382" cy="93383"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
@@ -14076,13 +13247,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>643872</xdr:colOff>
+      <xdr:colOff>499797</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>45415</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>737254</xdr:colOff>
+      <xdr:colOff>593179</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>138798</xdr:rowOff>
     </xdr:to>
@@ -14099,7 +13270,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2758422" y="2874340"/>
+          <a:off x="2620910" y="1886381"/>
           <a:ext cx="93382" cy="93383"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
@@ -14139,13 +13310,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>786136</xdr:colOff>
+      <xdr:colOff>642061</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>46796</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>879518</xdr:colOff>
+      <xdr:colOff>735443</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>140179</xdr:rowOff>
     </xdr:to>
@@ -14162,7 +13333,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2900686" y="2875721"/>
+          <a:off x="2763174" y="1887762"/>
           <a:ext cx="93382" cy="93383"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
@@ -14328,37 +13499,37 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>502959</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>47293</xdr:rowOff>
+      <xdr:colOff>50260</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>41962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>605680</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>140675</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="263" name="Rectangle 262">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8DB50B5-81B9-43AF-9822-CBC19328ECF7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1641313" y="2889305"/>
-          <a:ext cx="102721" cy="93382"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FF7D2D"/>
+      <xdr:colOff>143642</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>135345</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="265" name="Isosceles Triangle 264">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FC53144-466F-43E3-9C9B-7FEEA11455C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1186857" y="2075029"/>
+          <a:ext cx="93382" cy="93383"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="002060"/>
         </a:solidFill>
       </xdr:spPr>
       <xdr:style>
@@ -14391,37 +13562,37 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>194335</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>41962</xdr:rowOff>
+      <xdr:colOff>188997</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>40844</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>287717</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>135345</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="265" name="Isosceles Triangle 264">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FC53144-466F-43E3-9C9B-7FEEA11455C8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1327810" y="3061387"/>
+      <xdr:colOff>282379</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>134227</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="271" name="Isosceles Triangle 270">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56BF49AD-8D18-4E9E-90CE-344C3F74601E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1325594" y="2073911"/>
           <a:ext cx="93382" cy="93383"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="002060"/>
+          <a:srgbClr val="7030A0"/>
         </a:solidFill>
       </xdr:spPr>
       <xdr:style>
@@ -14454,76 +13625,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>333072</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>40844</xdr:rowOff>
+      <xdr:colOff>331261</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>44294</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>426454</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>134227</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="271" name="Isosceles Triangle 270">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56BF49AD-8D18-4E9E-90CE-344C3F74601E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1466547" y="3060269"/>
-          <a:ext cx="93382" cy="93383"/>
-        </a:xfrm>
-        <a:prstGeom prst="triangle">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="7030A0"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>475336</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>44294</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>568718</xdr:colOff>
+      <xdr:colOff>424643</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>137677</xdr:rowOff>
     </xdr:to>
@@ -14540,7 +13648,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1608811" y="3063719"/>
+          <a:off x="1467858" y="2077361"/>
           <a:ext cx="93382" cy="93383"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
@@ -14645,15 +13753,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>802765</xdr:colOff>
+      <xdr:colOff>656974</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>46311</xdr:rowOff>
+      <xdr:rowOff>50936</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>896147</xdr:colOff>
+      <xdr:colOff>750356</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>139694</xdr:rowOff>
+      <xdr:rowOff>144319</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -14668,7 +13776,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1941119" y="2888323"/>
+          <a:off x="1787749" y="1879532"/>
           <a:ext cx="93382" cy="93383"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
@@ -14708,15 +13816,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>45212</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>41576</xdr:rowOff>
+      <xdr:colOff>799062</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>51764</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>138593</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>134959</xdr:rowOff>
+      <xdr:colOff>892443</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>145147</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -14731,7 +13839,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1178687" y="3061001"/>
+          <a:off x="1929837" y="1880360"/>
           <a:ext cx="93381" cy="93383"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
@@ -14771,15 +13879,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>654003</xdr:colOff>
+      <xdr:colOff>508212</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>40489</xdr:rowOff>
+      <xdr:rowOff>45114</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>747385</xdr:colOff>
+      <xdr:colOff>601594</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>136628</xdr:rowOff>
+      <xdr:rowOff>141253</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -14794,7 +13902,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1792357" y="2882501"/>
+          <a:off x="1638987" y="1873710"/>
           <a:ext cx="93382" cy="96139"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
@@ -14826,80 +13934,6 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>194388</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>85530</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>785326</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>124407</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8766508-549A-4440-81FA-DBE5E59E0DBB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="194388" y="4463142"/>
-          <a:ext cx="1749489" cy="995265"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFF00"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>I think we need to make explanation of N vs n more visible</a:t>
-          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -18257,513 +17291,443 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" customWidth="1"/>
     <col min="3" max="8" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.21875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
     <col min="10" max="12" width="14.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="45"/>
+      <c r="A1" s="69" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="71"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="56" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="56" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" s="50" t="s">
+      <c r="A2" s="78" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="79"/>
+      <c r="C2" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="82" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="76" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="72" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="72" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="72" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="72" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="K2" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="46" t="s">
+      <c r="L2" s="74" t="s">
         <v>66</v>
-      </c>
-      <c r="H2" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="K2" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="L2" s="48" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="54"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="49"/>
+      <c r="A3" s="80"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="75"/>
     </row>
     <row r="4" spans="1:12" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="63"/>
-      <c r="B4" s="29" t="s">
+      <c r="A4" s="25"/>
+      <c r="B4" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="15" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="64"/>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" s="13" t="s">
+      <c r="C5" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J5" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="L5" s="31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="21" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="64"/>
+      <c r="B6" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="82" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="83" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="84" t="s">
-        <v>87</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="88" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="64"/>
-      <c r="B6" s="85" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="86" t="s">
-        <v>96</v>
-      </c>
-      <c r="D6" s="87" t="s">
-        <v>97</v>
-      </c>
-      <c r="E6" s="86" t="s">
-        <v>75</v>
-      </c>
-      <c r="F6" s="87" t="s">
-        <v>97</v>
-      </c>
-      <c r="G6" s="86" t="s">
-        <v>98</v>
-      </c>
-      <c r="H6" s="87" t="s">
-        <v>97</v>
-      </c>
-      <c r="I6" s="87" t="s">
-        <v>99</v>
-      </c>
-      <c r="J6" s="86" t="s">
-        <v>96</v>
-      </c>
-      <c r="K6" s="87" t="s">
-        <v>96</v>
-      </c>
-      <c r="L6" s="87" t="s">
-        <v>97</v>
+      <c r="C6" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="I6" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="J6" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="K6" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="L6" s="39" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="64"/>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="34">
         <v>0</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="35">
         <v>0</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="34">
         <v>0.02</v>
       </c>
-      <c r="F7" s="42">
+      <c r="F7" s="36">
         <v>0.27</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="36">
         <v>0.11</v>
       </c>
-      <c r="H7" s="42">
+      <c r="H7" s="36">
         <v>0.38</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="36">
         <v>0.1</v>
       </c>
-      <c r="J7" s="42">
+      <c r="J7" s="36">
         <v>0.35</v>
       </c>
-      <c r="K7" s="26">
+      <c r="K7" s="37">
         <v>0.19</v>
       </c>
-      <c r="L7" s="27">
+      <c r="L7" s="38">
         <v>0.42</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="64"/>
-      <c r="B8" s="39" t="s">
-        <v>100</v>
+    <row r="8" spans="1:12" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="65"/>
+      <c r="B8" s="67" t="s">
+        <v>86</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="D8" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="H8" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="I8" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="J8" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="K8" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="L8" s="35" t="s">
-        <v>85</v>
+        <v>89</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="87" t="s">
+        <v>97</v>
+      </c>
+      <c r="J8" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="K8" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="L8" s="42" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="64"/>
-      <c r="B9" s="89" t="s">
-        <v>100</v>
-      </c>
-      <c r="C9" s="91"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="93"/>
-      <c r="L9" s="94"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="55"/>
     </row>
     <row r="10" spans="1:12" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="38"/>
-      <c r="B10" s="90"/>
-      <c r="C10" s="92"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="72"/>
-      <c r="I10" s="72"/>
-      <c r="J10" s="72"/>
-      <c r="K10" s="72"/>
-      <c r="L10" s="95"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="56"/>
     </row>
     <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="68" t="s">
+      <c r="A12" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="70"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="45"/>
     </row>
     <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="68" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="69"/>
-      <c r="I13" s="69"/>
-      <c r="J13" s="69"/>
-      <c r="K13" s="69"/>
-      <c r="L13" s="70"/>
+      <c r="A13" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="45"/>
     </row>
     <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.3">
-      <c r="A14" s="79" t="s">
-        <v>83</v>
-      </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="80"/>
-      <c r="H14" s="80"/>
-      <c r="I14" s="80"/>
-      <c r="J14" s="80"/>
-      <c r="K14" s="80"/>
-      <c r="L14" s="81"/>
+      <c r="A14" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="48"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="65" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" s="66"/>
-      <c r="C15" s="66"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="66"/>
-      <c r="I15" s="66"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="66"/>
-      <c r="L15" s="67"/>
+      <c r="A15" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="59"/>
+      <c r="L15" s="60"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="B16" s="66"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="66"/>
-      <c r="I16" s="66"/>
-      <c r="J16" s="66"/>
-      <c r="K16" s="66"/>
-      <c r="L16" s="67"/>
+      <c r="A16" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="59"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="59"/>
+      <c r="K16" s="59"/>
+      <c r="L16" s="60"/>
     </row>
     <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.3">
-      <c r="A17" s="65" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" s="66"/>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="66"/>
-      <c r="J17" s="66"/>
-      <c r="K17" s="66"/>
-      <c r="L17" s="67"/>
+      <c r="A17" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="59"/>
+      <c r="L17" s="60"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="65" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="66"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="66"/>
-      <c r="I18" s="66"/>
-      <c r="J18" s="66"/>
-      <c r="K18" s="66"/>
-      <c r="L18" s="67"/>
+    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="60"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="65" t="s">
-        <v>82</v>
-      </c>
-      <c r="B19" s="66"/>
-      <c r="C19" s="66"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="66"/>
-      <c r="G19" s="66"/>
-      <c r="H19" s="66"/>
-      <c r="I19" s="66"/>
-      <c r="J19" s="66"/>
-      <c r="K19" s="66"/>
-      <c r="L19" s="67"/>
+    <row r="19" spans="1:12" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="62"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="62"/>
+      <c r="K19" s="62"/>
+      <c r="L19" s="63"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="65" t="s">
-        <v>90</v>
-      </c>
-      <c r="B20" s="66"/>
-      <c r="C20" s="66"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="66"/>
-      <c r="F20" s="66"/>
-      <c r="G20" s="66"/>
-      <c r="H20" s="66"/>
-      <c r="I20" s="66"/>
-      <c r="J20" s="66"/>
-      <c r="K20" s="66"/>
-      <c r="L20" s="67"/>
-    </row>
-    <row r="21" spans="1:12" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="76" t="s">
-        <v>91</v>
-      </c>
-      <c r="B21" s="77"/>
-      <c r="C21" s="77"/>
-      <c r="D21" s="77"/>
-      <c r="E21" s="77"/>
-      <c r="F21" s="77"/>
-      <c r="G21" s="77"/>
-      <c r="H21" s="77"/>
-      <c r="I21" s="77"/>
-      <c r="J21" s="77"/>
-      <c r="K21" s="77"/>
-      <c r="L21" s="78"/>
-    </row>
-    <row r="22" spans="1:12" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="58" t="s">
-        <v>94</v>
-      </c>
-      <c r="B22" s="59"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="59"/>
-      <c r="E22" s="59"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="59"/>
-      <c r="H22" s="59"/>
-      <c r="I22" s="59"/>
-      <c r="J22" s="59"/>
-      <c r="K22" s="59"/>
-      <c r="L22" s="60"/>
-    </row>
-    <row r="23" spans="1:12" s="37" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="36"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="36"/>
+    <row r="20" spans="1:12" s="20" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="A19:L19"/>
-    <mergeCell ref="A20:L20"/>
-    <mergeCell ref="A21:L21"/>
-    <mergeCell ref="A13:L13"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="A12:L12"/>
-    <mergeCell ref="A18:L18"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="A15:L15"/>
-    <mergeCell ref="A22:L22"/>
+  <mergeCells count="33">
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
@@ -18776,6 +17740,24 @@
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="G2:G3"/>
+    <mergeCell ref="A18:L18"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="A15:L15"/>
+    <mergeCell ref="A19:L19"/>
+    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="A12:L12"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18788,599 +17770,599 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="210" workbookViewId="0">
+    <sheetView topLeftCell="A44" zoomScale="111" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="73" t="s">
+    <row r="1" spans="1:4" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="75"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="86"/>
     </row>
-    <row r="2" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="12"/>
-      <c r="B2" s="14" t="s">
+    <row r="2" spans="1:4" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9">
+    <row r="3" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="8">
         <v>1963</v>
       </c>
-      <c r="D3" s="11"/>
+      <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
+    <row r="4" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="2">
         <v>1971</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+    <row r="5" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>1976</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+    <row r="6" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="2">
         <v>1984</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+    <row r="7" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="2">
         <v>1987</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+    <row r="8" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="2">
         <v>1987</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+    <row r="9" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="2">
         <v>1988</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+    <row r="10" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="2">
         <v>1998</v>
       </c>
-      <c r="D10" s="6"/>
+      <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+    <row r="11" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="2">
         <v>1999</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
+    <row r="12" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="2">
         <v>1999</v>
       </c>
-      <c r="D12" s="6"/>
+      <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
+    <row r="13" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
         <v>11</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="2">
         <v>2002</v>
       </c>
-      <c r="D13" s="6"/>
+      <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+    <row r="14" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
         <v>12</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="2">
         <v>2002</v>
       </c>
-      <c r="D14" s="6"/>
+      <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+    <row r="15" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
         <v>13</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="2">
         <v>2005</v>
       </c>
-      <c r="D15" s="6"/>
+      <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
+    <row r="16" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
         <v>14</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="2">
         <v>2005</v>
       </c>
-      <c r="D16" s="6"/>
+      <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
+    <row r="17" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
         <v>15</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="2">
         <v>2005</v>
       </c>
-      <c r="D17" s="6"/>
+      <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
+    <row r="18" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
         <v>16</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="2">
         <v>2005</v>
       </c>
-      <c r="D18" s="6"/>
+      <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
+    <row r="19" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
         <v>17</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="2">
         <v>2006</v>
       </c>
-      <c r="D19" s="6"/>
+      <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
+    <row r="20" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
         <v>18</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="2">
         <v>2007</v>
       </c>
-      <c r="D20" s="6"/>
+      <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
+    <row r="21" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
         <v>19</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="2">
         <v>2007</v>
       </c>
-      <c r="D21" s="6"/>
+      <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
+    <row r="22" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
         <v>20</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="2">
         <v>2008</v>
       </c>
-      <c r="D22" s="6"/>
+      <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
+    <row r="23" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
         <v>21</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="2">
         <v>2008</v>
       </c>
-      <c r="D23" s="6"/>
+      <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
+    <row r="24" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
         <v>22</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="2">
         <v>2008</v>
       </c>
-      <c r="D24" s="6"/>
+      <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
+    <row r="25" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
         <v>23</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="2">
         <v>2009</v>
       </c>
-      <c r="D25" s="6"/>
+      <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
+    <row r="26" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
         <v>24</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="2">
         <v>2009</v>
       </c>
-      <c r="D26" s="6"/>
+      <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5">
+    <row r="27" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
         <v>25</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="2">
         <v>2010</v>
       </c>
-      <c r="D27" s="6"/>
+      <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5">
+    <row r="28" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
         <v>26</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="2">
         <v>2010</v>
       </c>
-      <c r="D28" s="6"/>
+      <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5">
+    <row r="29" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
         <v>27</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="2">
         <v>2011</v>
       </c>
-      <c r="D29" s="6"/>
+      <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="5">
+    <row r="30" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
         <v>28</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="2">
         <v>2011</v>
       </c>
-      <c r="D30" s="6"/>
+      <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="5">
+    <row r="31" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
         <v>29</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="2">
         <v>2011</v>
       </c>
-      <c r="D31" s="6"/>
+      <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="5">
+    <row r="32" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
         <v>30</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="2">
         <v>2012</v>
       </c>
-      <c r="D32" s="6"/>
+      <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="5">
+    <row r="33" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
         <v>31</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="2">
         <v>2013</v>
       </c>
-      <c r="D33" s="6"/>
+      <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5">
+    <row r="34" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
         <v>32</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="2">
         <v>2014</v>
       </c>
-      <c r="D34" s="6"/>
+      <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="5">
+    <row r="35" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
         <v>33</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="2">
         <v>2014</v>
       </c>
-      <c r="D35" s="6"/>
+      <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="5">
+    <row r="36" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
         <v>34</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="2">
         <v>2014</v>
       </c>
-      <c r="D36" s="6"/>
+      <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="5">
+    <row r="37" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
         <v>35</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="2">
         <v>2015</v>
       </c>
-      <c r="D37" s="6"/>
+      <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="5">
+    <row r="38" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
         <v>36</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="2">
         <v>2015</v>
       </c>
-      <c r="D38" s="6"/>
+      <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="5">
+    <row r="39" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
         <v>37</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="2">
         <v>2015</v>
       </c>
-      <c r="D39" s="6"/>
+      <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="5">
+    <row r="40" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
         <v>38</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C40" s="2">
         <v>2016</v>
       </c>
-      <c r="D40" s="6"/>
+      <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="5">
+    <row r="41" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
         <v>39</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="2">
         <v>2016</v>
       </c>
-      <c r="D41" s="6"/>
+      <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="5">
+    <row r="42" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
         <v>40</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42" s="2">
         <v>2016</v>
       </c>
-      <c r="D42" s="6"/>
+      <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="5">
+    <row r="43" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
         <v>41</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C43" s="4">
+      <c r="B43" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" s="2">
         <v>2016</v>
       </c>
-      <c r="D43" s="6"/>
+      <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="5">
+    <row r="44" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="3">
         <v>42</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C44" s="2">
         <v>2016</v>
       </c>
-      <c r="D44" s="6"/>
+      <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="5">
+    <row r="45" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="3">
         <v>43</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C45" s="2">
         <v>2017</v>
       </c>
-      <c r="D45" s="6"/>
+      <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="5">
+    <row r="46" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
         <v>44</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="4">
+      <c r="C46" s="2">
         <v>2017</v>
       </c>
-      <c r="D46" s="6"/>
+      <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="5">
+    <row r="47" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="3">
         <v>45</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C47" s="4">
+      <c r="C47" s="2">
         <v>2018</v>
       </c>
-      <c r="D47" s="6"/>
+      <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="5">
+    <row r="48" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="3">
         <v>46</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C48" s="4">
+      <c r="C48" s="2">
         <v>2018</v>
       </c>
-      <c r="D48" s="6"/>
+      <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="1:4" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="22">
+    <row r="49" spans="1:4" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="17">
         <v>47</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C49" s="7">
+      <c r="C49" s="5">
         <v>2018</v>
       </c>
-      <c r="D49" s="8"/>
+      <c r="D49" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>